<commit_message>
les tables individuels avec id (manque continents pour pays et voir HongKong S.A.R + identifiants attribués dans le jeu de données principal Data
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -5,18 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/274365e861f80480/Documents/MIASHS/L3/Projet/Projet_L3/Données/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/274365e861f80480/Documents/MIASHS/L3/Projet/Projet_L3/Projet-L3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="11_AD4D9D64A577C15A4A541827889D7A045BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0668F0E9-6154-41DD-B956-44ACC2E82086}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="11_AD4D9D64A577C15A4A541827889D7A045BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7537DDD3-B54B-411D-9519-BC1F950928A6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pays" sheetId="1" r:id="rId1"/>
     <sheet name="Contient" sheetId="3" r:id="rId2"/>
-    <sheet name="Année" sheetId="6" r:id="rId3"/>
-    <sheet name="Score" sheetId="7" r:id="rId4"/>
+    <sheet name="Region" sheetId="8" r:id="rId3"/>
+    <sheet name="Année" sheetId="6" r:id="rId4"/>
+    <sheet name="Score" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,16 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="185">
-  <si>
-    <t>IdPays</t>
-  </si>
-  <si>
-    <t>NomPays</t>
-  </si>
-  <si>
-    <t>IdContinent</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="200">
   <si>
     <t>Switzerland</t>
   </si>
@@ -540,9 +532,6 @@
     <t>Taiwan Province of China</t>
   </si>
   <si>
-    <t>Hong Kong S.A.R.</t>
-  </si>
-  <si>
     <t>Trinidad &amp; Tobago</t>
   </si>
   <si>
@@ -555,9 +544,6 @@
     <t>Gambia</t>
   </si>
   <si>
-    <t>NomContinent</t>
-  </si>
-  <si>
     <t>Europe</t>
   </si>
   <si>
@@ -567,31 +553,91 @@
     <t>Asia</t>
   </si>
   <si>
-    <t>Antarctica</t>
-  </si>
-  <si>
     <t>North America</t>
   </si>
   <si>
     <t>South America</t>
   </si>
   <si>
-    <t>Année</t>
-  </si>
-  <si>
     <t>Family</t>
   </si>
   <si>
-    <t>IdScore</t>
-  </si>
-  <si>
-    <t>NomScore</t>
-  </si>
-  <si>
-    <t>Economy</t>
-  </si>
-  <si>
-    <t>Trust</t>
+    <t>Hapiness Rank</t>
+  </si>
+  <si>
+    <t>Hapiness Score</t>
+  </si>
+  <si>
+    <t>Economy (GDP per Capita)</t>
+  </si>
+  <si>
+    <t>Health (Life Expectancy)</t>
+  </si>
+  <si>
+    <t>Freedom</t>
+  </si>
+  <si>
+    <t>Trust (Government Corruption)</t>
+  </si>
+  <si>
+    <t>Generosity</t>
+  </si>
+  <si>
+    <t>Social support</t>
+  </si>
+  <si>
+    <t>Australia and New Zealand</t>
+  </si>
+  <si>
+    <t>Central and Eastern Europe</t>
+  </si>
+  <si>
+    <t>Eastern Asia</t>
+  </si>
+  <si>
+    <t>Latin America and Caribbean</t>
+  </si>
+  <si>
+    <t>Middle East and Northern Africa</t>
+  </si>
+  <si>
+    <t>Southeastern Asia</t>
+  </si>
+  <si>
+    <t>Southern Asia</t>
+  </si>
+  <si>
+    <t>Sub-Saharan Africa</t>
+  </si>
+  <si>
+    <t>Western Europe</t>
+  </si>
+  <si>
+    <t>Nom_Region</t>
+  </si>
+  <si>
+    <t>Id_Region</t>
+  </si>
+  <si>
+    <t>Id_Score</t>
+  </si>
+  <si>
+    <t>Nom_Score</t>
+  </si>
+  <si>
+    <t>Annee</t>
+  </si>
+  <si>
+    <t>Nom_Continent</t>
+  </si>
+  <si>
+    <t>Id_Continent</t>
+  </si>
+  <si>
+    <t>Id_Pays</t>
+  </si>
+  <si>
+    <t>Nom_Pays</t>
   </si>
 </sst>
 </file>
@@ -909,10 +955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C170"/>
+  <dimension ref="A1:C169"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -924,13 +970,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>198</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>199</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -938,7 +984,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -946,7 +992,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -954,7 +1000,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -962,7 +1008,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -970,7 +1016,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -978,7 +1024,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -986,7 +1032,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -994,7 +1040,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1002,7 +1048,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1010,7 +1056,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -1018,7 +1064,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -1026,7 +1072,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -1034,7 +1080,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -1042,7 +1088,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -1050,7 +1096,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -1058,7 +1104,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -1066,7 +1112,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -1074,7 +1120,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -1082,7 +1128,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -1090,7 +1136,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -1098,7 +1144,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -1106,7 +1152,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -1114,7 +1160,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -1122,7 +1168,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -1130,7 +1176,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -1138,7 +1184,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -1146,7 +1192,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -1154,7 +1200,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -1162,7 +1208,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -1170,7 +1216,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -1178,7 +1224,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -1186,7 +1232,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -1194,7 +1240,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -1202,7 +1248,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -1210,7 +1256,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
@@ -1218,7 +1264,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
@@ -1226,7 +1272,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
@@ -1234,7 +1280,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
@@ -1242,7 +1288,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
@@ -1250,7 +1296,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
@@ -1258,7 +1304,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
@@ -1266,7 +1312,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
@@ -1274,7 +1320,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
@@ -1282,7 +1328,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
@@ -1290,7 +1336,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
@@ -1298,7 +1344,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
@@ -1306,7 +1352,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
@@ -1314,7 +1360,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
@@ -1322,7 +1368,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
@@ -1330,7 +1376,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
@@ -1338,7 +1384,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
@@ -1346,7 +1392,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
@@ -1354,7 +1400,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
@@ -1362,7 +1408,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
@@ -1370,7 +1416,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
@@ -1378,7 +1424,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
@@ -1386,7 +1432,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
@@ -1394,7 +1440,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
@@ -1402,7 +1448,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
@@ -1410,7 +1456,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>167</v>
+        <v>102</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
@@ -1418,7 +1464,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
@@ -1426,7 +1472,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
@@ -1434,7 +1480,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
@@ -1442,7 +1488,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
@@ -1450,7 +1496,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
@@ -1458,7 +1504,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
@@ -1466,7 +1512,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
@@ -1474,7 +1520,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
@@ -1482,7 +1528,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>52</v>
+        <v>149</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
@@ -1490,7 +1536,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>152</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
@@ -1498,7 +1544,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
@@ -1506,7 +1552,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>48</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
@@ -1514,7 +1560,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
@@ -1522,7 +1568,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>56</v>
+        <v>123</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
@@ -1530,7 +1576,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
@@ -1538,7 +1584,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>71</v>
+        <v>38</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
@@ -1546,7 +1592,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>41</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
@@ -1554,7 +1600,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
@@ -1562,7 +1608,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
@@ -1570,7 +1616,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
@@ -1578,7 +1624,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
@@ -1586,7 +1632,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
@@ -1594,7 +1640,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>117</v>
+        <v>62</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
@@ -1602,7 +1648,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
@@ -1610,7 +1656,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
@@ -1618,7 +1664,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
@@ -1626,7 +1672,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>94</v>
+        <v>145</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
@@ -1634,7 +1680,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
@@ -1642,7 +1688,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
@@ -1650,7 +1696,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
@@ -1658,7 +1704,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>139</v>
+        <v>36</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
@@ -1666,7 +1712,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>39</v>
+        <v>122</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
@@ -1674,7 +1720,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>125</v>
+        <v>70</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
@@ -1682,7 +1728,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>73</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
@@ -1690,7 +1736,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
@@ -1698,7 +1744,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>54</v>
+        <v>98</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
@@ -1706,7 +1752,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
@@ -1714,7 +1760,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
@@ -1722,7 +1768,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
@@ -1730,7 +1776,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>95</v>
+        <v>127</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
@@ -1738,7 +1784,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
@@ -1746,7 +1792,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>164</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
@@ -1754,7 +1800,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>122</v>
+        <v>6</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
@@ -1762,7 +1808,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
@@ -1770,7 +1816,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
@@ -1778,7 +1824,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
@@ -1786,7 +1832,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>145</v>
+        <v>77</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
@@ -1794,7 +1840,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
@@ -1802,7 +1848,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
@@ -1810,7 +1856,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
@@ -1818,7 +1864,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>169</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
@@ -1826,7 +1872,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
@@ -1834,7 +1880,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
@@ -1842,7 +1888,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
@@ -1850,7 +1896,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>109</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
@@ -1858,7 +1904,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
@@ -1866,7 +1912,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
@@ -1874,7 +1920,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
@@ -1882,7 +1928,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>92</v>
+        <v>59</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
@@ -1890,7 +1936,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
@@ -1898,7 +1944,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
@@ -1906,7 +1952,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>160</v>
+        <v>27</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
@@ -1914,7 +1960,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
@@ -1922,7 +1968,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
@@ -1930,7 +1976,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>66</v>
+        <v>152</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
@@ -1938,7 +1984,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>155</v>
+        <v>34</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
@@ -1946,7 +1992,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>37</v>
+        <v>140</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
@@ -1954,7 +2000,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>143</v>
+        <v>86</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
@@ -1962,7 +2008,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>89</v>
+        <v>121</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
@@ -1970,7 +2016,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>124</v>
+        <v>23</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
@@ -1978,7 +2024,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
@@ -1986,7 +2032,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
@@ -1994,7 +2040,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>57</v>
+        <v>159</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
@@ -2002,7 +2048,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
@@ -2010,7 +2056,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>163</v>
+        <v>111</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
@@ -2018,7 +2064,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>114</v>
+        <v>46</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
@@ -2026,7 +2072,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>49</v>
+        <v>162</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
@@ -2034,7 +2080,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>165</v>
+        <v>35</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
@@ -2042,7 +2088,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>38</v>
+        <v>130</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
@@ -2050,7 +2096,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
@@ -2058,7 +2104,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>119</v>
+        <v>39</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
@@ -2066,7 +2112,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>42</v>
+        <v>99</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
@@ -2074,7 +2120,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>102</v>
+        <v>7</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
@@ -2082,7 +2128,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
@@ -2090,7 +2136,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>3</v>
+        <v>154</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
@@ -2098,7 +2144,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>157</v>
+        <v>37</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
@@ -2106,7 +2152,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>40</v>
+        <v>163</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
@@ -2114,7 +2160,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
@@ -2122,7 +2168,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>107</v>
+        <v>144</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
@@ -2130,7 +2176,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>147</v>
+        <v>33</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
@@ -2138,7 +2184,7 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>36</v>
+        <v>156</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
@@ -2146,7 +2192,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
@@ -2154,7 +2200,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>168</v>
+        <v>40</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
@@ -2162,7 +2208,7 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>43</v>
+        <v>105</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
@@ -2170,7 +2216,7 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
@@ -2178,7 +2224,7 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
@@ -2186,7 +2232,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
@@ -2194,7 +2240,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
@@ -2202,7 +2248,7 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>112</v>
+        <v>19</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
@@ -2210,7 +2256,7 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
@@ -2218,7 +2264,7 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
@@ -2226,7 +2272,7 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
@@ -2234,7 +2280,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
@@ -2242,7 +2288,7 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
@@ -2250,7 +2296,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
@@ -2258,7 +2304,7 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>77</v>
+        <v>134</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
@@ -2266,7 +2312,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>137</v>
+        <v>84</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
@@ -2274,15 +2320,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A170">
-        <v>169</v>
-      </c>
-      <c r="B170" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2292,20 +2330,245 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296D7ADF-BA11-4E98-866D-5EC617A7089E}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069BB508-CAE5-4288-A02C-FC738EC1705B}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>186</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C8F369-9484-43A3-B5B8-BCE1C997C6FC}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1F897A-94B2-4410-A583-55B89C03780E}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>193</v>
       </c>
       <c r="B1" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2313,7 +2576,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2321,7 +2584,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2329,7 +2592,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2337,7 +2600,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2345,7 +2608,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -2353,7 +2616,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -2361,90 +2624,23 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>178</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C8F369-9484-43A3-B5B8-BCE1C997C6FC}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>2016</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>2015</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF1F897A-94B2-4410-A583-55B89C03780E}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>181</v>
-      </c>
-      <c r="B1" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
le excel que mathis n'a pas réussi à push
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/274365e861f80480/Documents/MIASHS/L3/Projet/Projet_L3/Projet-L3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="11_AD4D9D64A577C15A4A541827889D7A045BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7537DDD3-B54B-411D-9519-BC1F950928A6}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="11_AD4D9D64A577C15A4A541827889D7A045BDEDD8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D51855B-1E5C-4635-B1F8-4BC7432524DC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pays" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="201">
   <si>
     <t>Switzerland</t>
   </si>
@@ -638,6 +638,9 @@
   </si>
   <si>
     <t>Nom_Pays</t>
+  </si>
+  <si>
+    <t>Hong Kong S.A.R.</t>
   </si>
 </sst>
 </file>
@@ -955,10 +958,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C169"/>
+  <dimension ref="A1:C170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -986,6 +989,9 @@
       <c r="B2" t="s">
         <v>151</v>
       </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -993,6 +999,9 @@
       </c>
       <c r="B3" t="s">
         <v>93</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1002,6 +1011,9 @@
       <c r="B4" t="s">
         <v>67</v>
       </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -1009,6 +1021,9 @@
       </c>
       <c r="B5" t="s">
         <v>135</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1018,6 +1033,9 @@
       <c r="B6" t="s">
         <v>29</v>
       </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -1026,6 +1044,9 @@
       <c r="B7" t="s">
         <v>125</v>
       </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
@@ -1034,6 +1055,9 @@
       <c r="B8" t="s">
         <v>9</v>
       </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
@@ -1042,6 +1066,9 @@
       <c r="B9" t="s">
         <v>12</v>
       </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
@@ -1050,6 +1077,9 @@
       <c r="B10" t="s">
         <v>79</v>
       </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
@@ -1058,6 +1088,9 @@
       <c r="B11" t="s">
         <v>48</v>
       </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
@@ -1066,6 +1099,9 @@
       <c r="B12" t="s">
         <v>107</v>
       </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
@@ -1074,6 +1110,9 @@
       <c r="B13" t="s">
         <v>58</v>
       </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
@@ -1082,6 +1121,9 @@
       <c r="B14" t="s">
         <v>18</v>
       </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
@@ -1090,6 +1132,9 @@
       <c r="B15" t="s">
         <v>158</v>
       </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
@@ -1098,1229 +1143,1702 @@
       <c r="B16" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C53">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C58">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C59">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C67">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C77">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C87">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C90">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C92">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C96">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C97">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C101">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C104">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C105">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C106">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
       <c r="B107" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>
       <c r="B109" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C109">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>109</v>
       </c>
       <c r="B110" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C110">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>110</v>
       </c>
       <c r="B111" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C111">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>111</v>
       </c>
       <c r="B112" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C112">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>112</v>
       </c>
       <c r="B113" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
       <c r="B114" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C114">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
       <c r="B115" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C115">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
       <c r="B116" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C116">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>116</v>
       </c>
       <c r="B117" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C117">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>117</v>
       </c>
       <c r="B118" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C118">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>118</v>
       </c>
       <c r="B119" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C119">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>119</v>
       </c>
       <c r="B120" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C120">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
       <c r="B121" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C121">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>121</v>
       </c>
       <c r="B122" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C122">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>122</v>
       </c>
       <c r="B123" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C123">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>123</v>
       </c>
       <c r="B124" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C124">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>124</v>
       </c>
       <c r="B125" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C125">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>125</v>
       </c>
       <c r="B126" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>126</v>
       </c>
       <c r="B127" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>127</v>
       </c>
       <c r="B128" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>128</v>
       </c>
       <c r="B129" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C129">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>129</v>
       </c>
       <c r="B130" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>130</v>
       </c>
       <c r="B131" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>131</v>
       </c>
       <c r="B132" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C132">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>132</v>
       </c>
       <c r="B133" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C133">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>133</v>
       </c>
       <c r="B134" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>134</v>
       </c>
       <c r="B135" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>135</v>
       </c>
       <c r="B136" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>136</v>
       </c>
       <c r="B137" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>137</v>
       </c>
       <c r="B138" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>138</v>
       </c>
       <c r="B139" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C139">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>139</v>
       </c>
       <c r="B140" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C140">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>140</v>
       </c>
       <c r="B141" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>141</v>
       </c>
       <c r="B142" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C142">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>142</v>
       </c>
       <c r="B143" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>143</v>
       </c>
       <c r="B144" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C144">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>144</v>
       </c>
       <c r="B145" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C145">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>145</v>
       </c>
       <c r="B146" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C146">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>146</v>
       </c>
       <c r="B147" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>147</v>
       </c>
       <c r="B148" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C148">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>148</v>
       </c>
       <c r="B149" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>149</v>
       </c>
       <c r="B150" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>150</v>
       </c>
       <c r="B151" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>151</v>
       </c>
       <c r="B152" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>152</v>
       </c>
       <c r="B153" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C153">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>153</v>
       </c>
       <c r="B154" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C154">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>154</v>
       </c>
       <c r="B155" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>155</v>
       </c>
       <c r="B156" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>156</v>
       </c>
       <c r="B157" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>157</v>
       </c>
       <c r="B158" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>158</v>
       </c>
       <c r="B159" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C159">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>159</v>
       </c>
       <c r="B160" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C160">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>160</v>
       </c>
       <c r="B161" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C161">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>161</v>
       </c>
       <c r="B162" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C162">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>162</v>
       </c>
       <c r="B163" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C163">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>163</v>
       </c>
       <c r="B164" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>164</v>
       </c>
       <c r="B165" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C165">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>165</v>
       </c>
       <c r="B166" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C166">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>166</v>
       </c>
       <c r="B167" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>167</v>
       </c>
       <c r="B168" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>168</v>
       </c>
       <c r="B169" t="s">
         <v>113</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170" t="s">
+        <v>200</v>
+      </c>
+      <c r="C170">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -2332,8 +2850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296D7ADF-BA11-4E98-866D-5EC617A7089E}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>